<commit_message>
Got IX service working.
</commit_message>
<xml_diff>
--- a/doc-engine-core/src/test/resources/content-export.xlsx
+++ b/doc-engine-core/src/test/resources/content-export.xlsx
@@ -8886,22 +8886,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N1142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>